<commit_message>
KPMP-1828: Add data type to switches. Fix typo in master
</commit_message>
<xml_diff>
--- a/validationScripts/MetadataMaster.xlsx
+++ b/validationScripts/MetadataMaster.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachw\Documents\GitRepos\metadata-consumer\validationScripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24477DD0-19D0-4BDC-9697-EF839AE2D730}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CA37F8-1A9B-45F4-B273-4CCBA87BA518}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Information" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="580">
   <si>
     <t>Associated File Type</t>
   </si>
@@ -1790,9 +1790,6 @@
     <t>CryosectioningDate</t>
   </si>
   <si>
-    <t>TissueSegmentionDissociationDate</t>
-  </si>
-  <si>
     <t>RNAIsolationDate</t>
   </si>
   <si>
@@ -1962,6 +1959,12 @@
   </si>
   <si>
     <t>NumberofCellsSequencedPostQC</t>
+  </si>
+  <si>
+    <t>Tissue Segmentation / Dissociation Date</t>
+  </si>
+  <si>
+    <t>TissueSegmentationDissociationDate</t>
   </si>
 </sst>
 </file>
@@ -3985,10 +3988,10 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4105,7 +4108,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>81</v>
+        <v>578</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>82</v>
@@ -4133,7 +4136,7 @@
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>521</v>
+        <v>579</v>
       </c>
       <c r="O3" s="9">
         <v>43209</v>
@@ -4175,7 +4178,7 @@
         <v>24</v>
       </c>
       <c r="M4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="O4" s="9">
         <v>43210</v>
@@ -4219,7 +4222,7 @@
         <v>24</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>88</v>
@@ -4263,7 +4266,7 @@
         <v>96</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>97</v>
@@ -4305,7 +4308,7 @@
         <v>96</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>100</v>
@@ -4346,7 +4349,7 @@
         <v>24</v>
       </c>
       <c r="M8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="12.75">
@@ -4384,7 +4387,7 @@
         <v>24</v>
       </c>
       <c r="M9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="12.75">
@@ -4421,7 +4424,7 @@
         <v>96</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="N10" s="16"/>
       <c r="O10" s="14"/>
@@ -4461,7 +4464,7 @@
         <v>24</v>
       </c>
       <c r="M11" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="O11" s="1"/>
     </row>
@@ -4501,7 +4504,7 @@
         <v>24</v>
       </c>
       <c r="M12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O12" s="1">
         <v>361644</v>
@@ -4543,7 +4546,7 @@
         <v>24</v>
       </c>
       <c r="M13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O13" s="1"/>
     </row>
@@ -4583,7 +4586,7 @@
         <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -4624,7 +4627,7 @@
         <v>24</v>
       </c>
       <c r="M15" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>121</v>
@@ -4667,7 +4670,7 @@
         <v>96</v>
       </c>
       <c r="M16" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -4707,7 +4710,7 @@
         <v>24</v>
       </c>
       <c r="M17" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="O17" s="1">
         <v>2.2999999999999998</v>
@@ -4749,7 +4752,7 @@
         <v>24</v>
       </c>
       <c r="M18" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="O18" s="1">
         <v>83</v>
@@ -4791,7 +4794,7 @@
         <v>24</v>
       </c>
       <c r="M19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="O19" s="1"/>
     </row>
@@ -4828,7 +4831,7 @@
         <v>24</v>
       </c>
       <c r="M20" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="O20" s="1"/>
     </row>
@@ -4865,7 +4868,7 @@
         <v>24</v>
       </c>
       <c r="M21" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="O21" s="1"/>
     </row>
@@ -4904,7 +4907,7 @@
         <v>24</v>
       </c>
       <c r="M22" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="O22" s="1">
         <v>30137</v>
@@ -4946,7 +4949,7 @@
         <v>24</v>
       </c>
       <c r="M23" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O23" s="1"/>
     </row>
@@ -4983,7 +4986,7 @@
         <v>24</v>
       </c>
       <c r="M24" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="O24" s="1"/>
     </row>
@@ -5020,7 +5023,7 @@
         <v>24</v>
       </c>
       <c r="M25" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>161</v>
@@ -5061,7 +5064,7 @@
         <v>24</v>
       </c>
       <c r="M26" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>163</v>
@@ -5102,7 +5105,7 @@
         <v>24</v>
       </c>
       <c r="M27" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="12.75">
@@ -5141,7 +5144,7 @@
         <v>96</v>
       </c>
       <c r="M28" s="16" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
@@ -5182,7 +5185,7 @@
         <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>182</v>
@@ -5223,7 +5226,7 @@
         <v>24</v>
       </c>
       <c r="M30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>186</v>
@@ -5264,7 +5267,7 @@
         <v>24</v>
       </c>
       <c r="M31" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="12.75">
@@ -5299,7 +5302,7 @@
         <v>24</v>
       </c>
       <c r="M32" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="12.75">
@@ -5337,7 +5340,7 @@
         <v>24</v>
       </c>
       <c r="M33" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="12.75">
@@ -5375,7 +5378,7 @@
         <v>96</v>
       </c>
       <c r="M34" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="12.75">
@@ -5413,7 +5416,7 @@
         <v>24</v>
       </c>
       <c r="M35" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>201</v>
@@ -5452,7 +5455,7 @@
         <v>24</v>
       </c>
       <c r="M36" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="12.75">
@@ -5491,7 +5494,7 @@
         <v>24</v>
       </c>
       <c r="M37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="12.75">
@@ -5527,7 +5530,7 @@
         <v>24</v>
       </c>
       <c r="M38" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="12.75">
@@ -5565,7 +5568,7 @@
         <v>24</v>
       </c>
       <c r="M39" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="12.75">
@@ -5603,7 +5606,7 @@
         <v>24</v>
       </c>
       <c r="M40" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="12.75">
@@ -5639,7 +5642,7 @@
         <v>24</v>
       </c>
       <c r="M41" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="P41" s="1"/>
     </row>
@@ -5679,7 +5682,7 @@
         <v>96</v>
       </c>
       <c r="M42" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N42" s="16"/>
       <c r="O42" s="16"/>
@@ -5721,7 +5724,7 @@
         <v>24</v>
       </c>
       <c r="M43" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="12.75">
@@ -5760,7 +5763,7 @@
         <v>24</v>
       </c>
       <c r="M44" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="12.75">
@@ -5799,7 +5802,7 @@
         <v>24</v>
       </c>
       <c r="M45" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="12.75">
@@ -5835,7 +5838,7 @@
         <v>24</v>
       </c>
       <c r="M46" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="12.75">
@@ -5871,7 +5874,7 @@
         <v>24</v>
       </c>
       <c r="M47" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="12.75">
@@ -5910,7 +5913,7 @@
         <v>24</v>
       </c>
       <c r="M48" s="16" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="N48" s="16"/>
       <c r="O48" s="16"/>
@@ -5952,7 +5955,7 @@
         <v>24</v>
       </c>
       <c r="M49" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="12.75">
@@ -5988,7 +5991,7 @@
         <v>96</v>
       </c>
       <c r="M50" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="12.75">
@@ -6024,7 +6027,7 @@
         <v>24</v>
       </c>
       <c r="M51" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="12.75">
@@ -6062,7 +6065,7 @@
         <v>24</v>
       </c>
       <c r="M52" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="12.75">
@@ -6098,7 +6101,7 @@
         <v>24</v>
       </c>
       <c r="M53" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="12.75">
@@ -6134,7 +6137,7 @@
         <v>24</v>
       </c>
       <c r="M54" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="12.75">
@@ -6170,7 +6173,7 @@
         <v>24</v>
       </c>
       <c r="M55" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="12.75">
@@ -6208,7 +6211,7 @@
         <v>24</v>
       </c>
       <c r="M56" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="12.75">
@@ -6246,7 +6249,7 @@
         <v>24</v>
       </c>
       <c r="M57" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="12.75">
@@ -6284,7 +6287,7 @@
         <v>24</v>
       </c>
       <c r="M58" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="12.75">
@@ -6322,7 +6325,7 @@
         <v>24</v>
       </c>
       <c r="M59" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="12.75">
@@ -6361,7 +6364,7 @@
         <v>96</v>
       </c>
       <c r="M60" s="16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="N60" s="16"/>
       <c r="O60" s="16"/>

</xml_diff>